<commit_message>
Network and GSEA updating
</commit_message>
<xml_diff>
--- a/tests/data/proteins/longitudinal_pdata.xlsx
+++ b/tests/data/proteins/longitudinal_pdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\omicscope\omicscope\tests\data\proteins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CD5F8A-E0DE-4E5E-AD7A-E3531D1DBBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6106D044-7230-4111-B72A-D0A5FC366259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{95A0D66F-0B16-43F7-9053-459AC203F225}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{95A0D66F-0B16-43F7-9053-459AC203F225}"/>
   </bookViews>
   <sheets>
     <sheet name="Independent" sheetId="1" r:id="rId1"/>
@@ -561,7 +561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62BA070D-AC61-4C33-9D68-7186420F4625}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -1268,11 +1268,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288D20AD-ECBC-4858-883D-9A01880AAC11}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1282,10 +1289,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>54</v>
@@ -1333,10 +1340,10 @@
         <v>53</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1350,10 +1357,10 @@
         <v>53</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -1367,10 +1374,10 @@
         <v>53</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -1384,10 +1391,10 @@
         <v>53</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -1401,10 +1408,10 @@
         <v>53</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1418,10 +1425,10 @@
         <v>53</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1435,10 +1442,10 @@
         <v>53</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -1452,10 +1459,10 @@
         <v>53</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -1469,10 +1476,10 @@
         <v>53</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -1486,10 +1493,10 @@
         <v>53</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -1503,10 +1510,10 @@
         <v>53</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1520,10 +1527,10 @@
         <v>53</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D15">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1537,10 +1544,10 @@
         <v>53</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D16">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E16">
         <v>2</v>
@@ -1554,10 +1561,10 @@
         <v>53</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D17">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -1571,10 +1578,10 @@
         <v>53</v>
       </c>
       <c r="C18">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D18">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E18">
         <v>3</v>
@@ -1588,10 +1595,10 @@
         <v>53</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D19">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E19">
         <v>3</v>
@@ -1605,10 +1612,10 @@
         <v>53</v>
       </c>
       <c r="C20">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D20">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1622,10 +1629,10 @@
         <v>53</v>
       </c>
       <c r="C21">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D21">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1639,10 +1646,10 @@
         <v>53</v>
       </c>
       <c r="C22">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D22">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E22">
         <v>2</v>
@@ -1656,10 +1663,10 @@
         <v>53</v>
       </c>
       <c r="C23">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D23">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E23">
         <v>2</v>
@@ -1673,10 +1680,10 @@
         <v>53</v>
       </c>
       <c r="C24">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D24">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E24">
         <v>3</v>
@@ -1690,10 +1697,10 @@
         <v>53</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D25">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E25">
         <v>3</v>
@@ -1707,10 +1714,10 @@
         <v>4</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D26">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E26">
         <v>4</v>
@@ -1724,10 +1731,10 @@
         <v>4</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D27">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E27">
         <v>4</v>
@@ -1741,10 +1748,10 @@
         <v>4</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D28">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E28">
         <v>5</v>
@@ -1758,10 +1765,10 @@
         <v>4</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D29">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E29">
         <v>5</v>
@@ -1775,10 +1782,10 @@
         <v>4</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D30">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E30">
         <v>6</v>
@@ -1792,10 +1799,10 @@
         <v>4</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D31">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E31">
         <v>6</v>
@@ -1809,10 +1816,10 @@
         <v>4</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D32">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E32">
         <v>4</v>
@@ -1826,10 +1833,10 @@
         <v>4</v>
       </c>
       <c r="C33">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D33">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E33">
         <v>4</v>
@@ -1843,10 +1850,10 @@
         <v>4</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D34">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="E34">
         <v>5</v>
@@ -1860,10 +1867,10 @@
         <v>4</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D35">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="E35">
         <v>5</v>
@@ -1877,10 +1884,10 @@
         <v>4</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D36">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E36">
         <v>6</v>
@@ -1894,10 +1901,10 @@
         <v>4</v>
       </c>
       <c r="C37">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D37">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E37">
         <v>6</v>
@@ -1911,10 +1918,10 @@
         <v>4</v>
       </c>
       <c r="C38">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D38">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E38">
         <v>4</v>
@@ -1928,10 +1935,10 @@
         <v>4</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D39">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E39">
         <v>4</v>
@@ -1945,10 +1952,10 @@
         <v>4</v>
       </c>
       <c r="C40">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D40">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E40">
         <v>5</v>
@@ -1962,10 +1969,10 @@
         <v>4</v>
       </c>
       <c r="C41">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D41">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E41">
         <v>5</v>
@@ -1979,10 +1986,10 @@
         <v>4</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D42">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="E42">
         <v>6</v>
@@ -1996,10 +2003,10 @@
         <v>4</v>
       </c>
       <c r="C43">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D43">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="E43">
         <v>6</v>
@@ -2013,10 +2020,10 @@
         <v>4</v>
       </c>
       <c r="C44">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D44">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E44">
         <v>4</v>
@@ -2030,10 +2037,10 @@
         <v>4</v>
       </c>
       <c r="C45">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D45">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E45">
         <v>4</v>
@@ -2047,10 +2054,10 @@
         <v>4</v>
       </c>
       <c r="C46">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D46">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E46">
         <v>5</v>
@@ -2064,10 +2071,10 @@
         <v>4</v>
       </c>
       <c r="C47">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D47">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E47">
         <v>5</v>
@@ -2081,10 +2088,10 @@
         <v>4</v>
       </c>
       <c r="C48">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D48">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E48">
         <v>6</v>
@@ -2098,10 +2105,10 @@
         <v>4</v>
       </c>
       <c r="C49">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D49">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E49">
         <v>6</v>
@@ -2113,21 +2120,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A7AC55A04AAE234C954FA09C434FB391" ma:contentTypeVersion="5" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="95303bc2901cc34184f795c32446e7c2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5d8c2e54-5123-4986-851c-3264d5158828" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="200bc172d5fdf9400889c226faaf7d17" ns3:_="">
     <xsd:import namespace="5d8c2e54-5123-4986-851c-3264d5158828"/>
@@ -2277,31 +2269,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8C67938-057A-45A0-8F81-F2654D918A45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5d8c2e54-5123-4986-851c-3264d5158828"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A873F1B-16CA-4C5A-A7C2-C76186C8D7DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0933C5FD-EB7C-44F7-AD61-85E4DDFAEC77}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2317,4 +2300,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A873F1B-16CA-4C5A-A7C2-C76186C8D7DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8C67938-057A-45A0-8F81-F2654D918A45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5d8c2e54-5123-4986-851c-3264d5158828"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>